<commit_message>
Ordenamiento general de archivos y procesos
Arreglos menores. Se agregan librerías a 02. Se corrige lectura de archivo con bases para excluir resultados. Se juntan SNU Privado y Estatal. Se diferencia base por tipo de culto (Católico vs Otro).
</commit_message>
<xml_diff>
--- a/analysis/data/bases.xlsx
+++ b/analysis/data/bases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\este.de.ahora\Documents\Dropbox\Pablo\Espacio de investigacion\_en-proceso\pilar\analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83F30C44-DE08-4AEA-B6BE-06EFF85A829E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE1635B3-54A5-4660-A591-C76D922EF471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-14780" windowWidth="26301" windowHeight="14169" xr2:uid="{0BF7A20E-7414-4DDB-BBC3-D15D5DFAFE24}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14169" xr2:uid="{0BF7A20E-7414-4DDB-BBC3-D15D5DFAFE24}"/>
   </bookViews>
   <sheets>
     <sheet name="db" sheetId="1" r:id="rId1"/>
@@ -63,12 +63,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="A10" authorId="0" shapeId="0" xr:uid="{5443E3E2-6B9D-4033-9A6B-03752C691F14}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Agregar farmacias y Sanatorios privados.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="93">
   <si>
     <t>db</t>
   </si>
@@ -181,9 +205,6 @@
     <t>Centros de Jubilados</t>
   </si>
   <si>
-    <t>Espacios religiosos</t>
-  </si>
-  <si>
     <t>ORGANIZACION</t>
   </si>
   <si>
@@ -208,9 +229,6 @@
     <t>Parques y Espacio verdes</t>
   </si>
   <si>
-    <t xml:space="preserve">      </t>
-  </si>
-  <si>
     <t>INICIAL_ESTATAL</t>
   </si>
   <si>
@@ -229,12 +247,6 @@
     <t>SECUNDARIO_PRIVADO</t>
   </si>
   <si>
-    <t xml:space="preserve">SNU_ESTATAL          </t>
-  </si>
-  <si>
-    <t>SNU_PRIVADO</t>
-  </si>
-  <si>
     <t>Nivel Primario Estatal</t>
   </si>
   <si>
@@ -253,12 +265,6 @@
     <t>Nivel Inicial Privado</t>
   </si>
   <si>
-    <t>Nivel SNU Estatal</t>
-  </si>
-  <si>
-    <t>Nivel SNU Privado</t>
-  </si>
-  <si>
     <t>Universidad</t>
   </si>
   <si>
@@ -289,9 +295,6 @@
     <t>Parada de colectivo de jurisdicción Municipal</t>
   </si>
   <si>
-    <t xml:space="preserve">EDIFICIO_RELIGIOSO </t>
-  </si>
-  <si>
     <t>POLICE</t>
   </si>
   <si>
@@ -301,9 +304,6 @@
     <t>Institución de Atención Médica de Gestión Estatal</t>
   </si>
   <si>
-    <t>EST_SERV</t>
-  </si>
-  <si>
     <t xml:space="preserve">FABRICA              </t>
   </si>
   <si>
@@ -343,9 +343,6 @@
     <t>Infraestructura</t>
   </si>
   <si>
-    <t xml:space="preserve">               </t>
-  </si>
-  <si>
     <t>TREN_EST</t>
   </si>
   <si>
@@ -353,6 +350,27 @@
   </si>
   <si>
     <t>Acceso a Autopista o vía principal</t>
+  </si>
+  <si>
+    <t>EST_SERVICIO</t>
+  </si>
+  <si>
+    <t>CULTO_OTRO</t>
+  </si>
+  <si>
+    <t>Centro Religioso Católico</t>
+  </si>
+  <si>
+    <t>Centro Religioso No-Católico (Evangelista)</t>
+  </si>
+  <si>
+    <t>CULTO_CATOLICO</t>
+  </si>
+  <si>
+    <t>SNU</t>
+  </si>
+  <si>
+    <t>Nivel SNU (Estatal y Privado)</t>
   </si>
 </sst>
 </file>
@@ -733,10 +751,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCF6E4DC-919E-4C5B-97D7-9C915E7F70B5}">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -746,7 +764,7 @@
     <col min="4" max="4" width="34.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -763,12 +781,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -780,12 +798,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -797,12 +815,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -814,12 +832,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -831,12 +849,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -848,12 +866,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B7" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -865,12 +883,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>91</v>
       </c>
       <c r="B8" t="s">
-        <v>61</v>
+        <v>92</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
@@ -882,12 +900,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
@@ -899,171 +917,168 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B10" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="B11" t="s">
-        <v>76</v>
+        <v>43</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="D11" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
-      <c r="H11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>77</v>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>84</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
       <c r="C12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" t="s">
         <v>40</v>
       </c>
-      <c r="D12" t="s">
-        <v>41</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E12" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>93</v>
+        <v>62</v>
       </c>
       <c r="B13" t="s">
-        <v>94</v>
+        <v>66</v>
       </c>
       <c r="C13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" t="s">
         <v>40</v>
-      </c>
-      <c r="D13" t="s">
-        <v>41</v>
       </c>
       <c r="E13" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B14" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" t="s">
         <v>40</v>
-      </c>
-      <c r="D14" t="s">
-        <v>41</v>
       </c>
       <c r="E14" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B15" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" t="s">
         <v>40</v>
-      </c>
-      <c r="D15" t="s">
-        <v>41</v>
       </c>
       <c r="E15" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="B16" t="s">
-        <v>70</v>
+        <v>41</v>
       </c>
       <c r="C16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" t="s">
         <v>40</v>
       </c>
-      <c r="D16" t="s">
-        <v>41</v>
-      </c>
-      <c r="E16" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>92</v>
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C17" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="D17" t="s">
-        <v>41</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="E17" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>88</v>
       </c>
       <c r="C18" t="s">
-        <v>15</v>
+        <v>78</v>
       </c>
       <c r="D18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E18" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
+        <v>89</v>
       </c>
       <c r="C19" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="D19" t="s">
         <v>32</v>
@@ -1072,9 +1087,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B20" t="s">
         <v>17</v>
@@ -1089,89 +1104,86 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B21" t="s">
         <v>28</v>
       </c>
       <c r="C21" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D21" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="E21">
         <v>1</v>
       </c>
-      <c r="H21" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" t="s">
         <v>81</v>
       </c>
-      <c r="B22" t="s">
-        <v>84</v>
-      </c>
-      <c r="C22" t="s">
-        <v>89</v>
-      </c>
       <c r="D22" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="E22">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B23" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C23" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D23" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="E23">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24" t="s">
+        <v>74</v>
+      </c>
+      <c r="C24" t="s">
         <v>79</v>
       </c>
-      <c r="B24" t="s">
+      <c r="D24" t="s">
         <v>82</v>
       </c>
-      <c r="C24" t="s">
-        <v>87</v>
-      </c>
-      <c r="D24" t="s">
-        <v>90</v>
-      </c>
       <c r="E24">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B25" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C25" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="D25" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -1189,7 +1201,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1386,10 +1398,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" t="s">
         <v>38</v>
-      </c>
-      <c r="B12" t="s">
-        <v>39</v>
       </c>
       <c r="C12" t="s">
         <v>31</v>
@@ -1403,16 +1415,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="E13" s="2">
         <v>1</v>

</xml_diff>